<commit_message>
Mid Level Python Test
</commit_message>
<xml_diff>
--- a/api/management/commands/cryptoexcel.xlsx
+++ b/api/management/commands/cryptoexcel.xlsx
@@ -424,7 +424,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,32 +467,640 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Bitcoin, Ethereum, Tether, BNB, USD Coin, XRP, Cardano, Dogecoin, Solana, Polygon, Polkadot, TRON, Litecoin, Binance USD, Shiba Inu, Avalanche, Dai, Wrapped Bitcoin, Chainlink, UNUS SED LEO</t>
+          <t>Bitcoin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BTC, ETH, USDT, BNB, USDC, XRP, ADA, DOGE, SOL, MATIC, DOT, TRX, LTC, BUSD, SHIB, AVAX, DAI, WBTC, LINK, LEO</t>
+          <t>BTC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$519,890,519,912, $220,751,144,457, $82,841,877,898, $48,308,214,611, $29,977,741,959, $22,065,907,039, $12,682,969,628, $9,982,108,918, $8,253,532,761, $7,874,818,434, $6,316,624,362, $6,258,359,506, $5,857,349,803, $5,616,012,148, $5,136,585,621, $4,975,454,239, $4,864,373,643, $4,154,124,104, $3,377,669,883, $3,256,769,938</t>
+          <t>$520,281,585,681</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>$26,837.03, $1,796.03, $1.00, $309.95, $1.00, $0.4257, $0.364, $0.07164, $20.87, $0.8514, $5.34, $0.06919, $80.34, $1.00, $0.000008713, $14.97, $0.9997, $26,799.11, $6.53, $3.50</t>
+          <t>$26,859.82</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>19,372,131 BTC, 122,910,443 ETH *, 82,797,235,449 USDT *, 155,860,056 BNB *, 29,975,346,921 USDC *, 51,837,820,505 XRP *, 34,844,746,976 ADA *, 139,329,366,384 DOGE, 395,476,214 SOL *, 9,249,469,069 MATIC *, 1,183,531,137 DOT *, 90,452,782,304 TRX *, 72,910,077 LTC, 5,614,434,149 BUSD *, 589,537,816,029,355 SHIB *, 332,304,876 AVAX *, 4,865,982,981 DAI *, 155,010 WBTC *, 517,099,970 LINK *, 930,386,731 LEO *</t>
+          <t>19,373,037 BTC</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>$13,579,284,679, $6,403,541,310, $20,871,433,415, $430,602,152, $2,768,230,164, $558,022,175, $177,961,738, $231,608,075, $313,852,048, $370,252,887, $100,775,255, $177,805,694, $382,268,177, $1,883,248,926, $111,905,802, $105,719,645, $128,087,231, $87,168,934, $141,675,175, $674,393</t>
+          <t>$9,221,300,540</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ethereum</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ETH</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>$222,072,570,877</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>$1,806.32</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>122,951,966 ETH *</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>$4,384,995,638</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Tether</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>USDT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>$82,829,940,350</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>$1.00</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>82,797,235,449 USDT *</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>$14,033,678,331</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BNB</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BNB</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>$48,677,456,991</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>$312.32</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>155,859,906 BNB *</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>$376,328,882</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>USD Coin</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>USDC</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>$29,969,145,629</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>$0.9998</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>29,974,410,122 USDC *</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>$1,729,040,340</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>XRP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>$22,148,386,271</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>$0.4273</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>51,837,820,505 XRP *</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>$341,159,960</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cardano</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ADA</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>$12,821,499,031</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>$0.3679</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>34,848,717,595 ADA *</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>$115,807,003</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Dogecoin</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DOGE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>$10,061,268,740</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>$0.07221</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>139,341,786,384 DOGE</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>$135,055,657</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Solana</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>SOL</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>$8,347,607,969</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>$21.11</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>395,475,347 SOL *</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>$203,660,082</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Polygon</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>MATIC</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>$7,913,517,471</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>$0.8556</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>9,249,469,069 MATIC *</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>$281,765,689</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Polkadot</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>DOT</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$6,359,741,244</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>$5.37</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1,183,866,812 DOT *</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>$74,782,117</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TRON</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>TRX</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>$6,283,070,567</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>$0.06947</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>90,444,632,098 TRX *</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>$144,998,974</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Litecoin</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>LTC</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>$5,963,818,206</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>$81.79</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>72,917,377 LTC</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>$301,328,798</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Binance USD</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BUSD</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$5,617,755,226</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>$1.00</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>5,614,434,149 BUSD *</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>$1,333,169,653</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Shiba Inu</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>SHIB</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>$5,185,957,972</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>$0.000008797</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>589,537,967,495,208 SHIB *</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>$80,178,932</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Avalanche</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>AVAX</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>$4,992,872,031</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>$15.02</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>332,452,841 AVAX *</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>$77,293,574</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Dai</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>DAI</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>$4,862,853,671</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>$1.00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>4,861,998,896 DAI *</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>$43,881,579</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Wrapped Bitcoin</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>WBTC</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>$4,173,675,088</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>$26,873.31</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>155,309 WBTC *</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>$59,968,312</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Chainlink</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>$3,385,987,203</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>$6.55</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>517,099,970 LINK *</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>$97,921,681</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>UNUS SED LEO</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>LEO</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>$3,334,772,110</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>$3.58</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>930,377,013 LEO *</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>$487,494</t>
         </is>
       </c>
     </row>

</xml_diff>